<commit_message>
Actualización del cronograma de proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/GoShop/Documentos/GS-CP.xlsx
+++ b/Desarrollo/GoShop/Documentos/GS-CP.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="185">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -110,10 +110,10 @@
     <t>Elaborar Plan de Fase</t>
   </si>
   <si>
-    <t>Documento de Plan de Fase 1</t>
-  </si>
-  <si>
-    <t>GS-PF-01.DOCX</t>
+    <t>Documento de Plan de Fase</t>
+  </si>
+  <si>
+    <t>GS-PF.DOCX</t>
   </si>
   <si>
     <t>Elaborar Plan de Iteración 1</t>
@@ -137,10 +137,10 @@
     <t>Especificar la Arquitectura y Diseño del Software</t>
   </si>
   <si>
-    <t>Documento de Arquitectura del Software 1</t>
-  </si>
-  <si>
-    <t>GS-AS-01.DOCX</t>
+    <t>Documento de Arquitectura del Software</t>
+  </si>
+  <si>
+    <t>GS-AS.DOCX</t>
   </si>
   <si>
     <t>Ipanaque J. (AS), Ramírez P. (UX)</t>
@@ -149,10 +149,10 @@
     <t>Proponer el diseño inicial de la Interface Web (UI)</t>
   </si>
   <si>
-    <t>Documento de Especificación de UI 1</t>
-  </si>
-  <si>
-    <t>GS-UI-01.DOCX</t>
+    <t>Documento de Especificación de UI</t>
+  </si>
+  <si>
+    <t>GS-UI.DOCX</t>
   </si>
   <si>
     <t>Ramírez P. (UX)</t>
@@ -161,19 +161,19 @@
     <t>Establecer estilos para la web</t>
   </si>
   <si>
-    <t>Documento de Guía de Estilos 1</t>
-  </si>
-  <si>
-    <t>GS-GE-01.DOCX</t>
+    <t>Documento de Guía de Estilos</t>
+  </si>
+  <si>
+    <t>GS-GE.DOCX</t>
   </si>
   <si>
     <t>Especificar el diseño de la Base de Datos</t>
   </si>
   <si>
-    <t>Documento de Especificación de la BD 1</t>
-  </si>
-  <si>
-    <t>GS-DEBD-01.DOCX</t>
+    <t>Documento de Especificación de la BD</t>
+  </si>
+  <si>
+    <t>GS-DEBD.DOCX</t>
   </si>
   <si>
     <t>Ames D.  (ABD), Ramírez P. (ABD)</t>
@@ -272,7 +272,10 @@
     <t>Codificación de requisito 1</t>
   </si>
   <si>
-    <t>*.py</t>
+    <t>Código del requisito 1</t>
+  </si>
+  <si>
+    <t>*.py, *.html, *.css, *.js</t>
   </si>
   <si>
     <t>Ames D. (DF), Cjumo J. (DB), Hinostroza G. (DB), Saenz C. (DF)</t>
@@ -281,7 +284,10 @@
     <t>Test de requisito 1</t>
   </si>
   <si>
-    <t>tests-01.py</t>
+    <t>Código de prueba unitaria del requisito 1</t>
+  </si>
+  <si>
+    <t>tests_01.py</t>
   </si>
   <si>
     <t>Castillo C. (T), Saenz J. (T)</t>
@@ -290,22 +296,31 @@
     <t>Codificación de requisito 2</t>
   </si>
   <si>
-    <t>*.html</t>
+    <t>Código del requisito 2</t>
   </si>
   <si>
     <t>Test de requisito 2</t>
   </si>
   <si>
-    <t>tests-02.py</t>
+    <t>Código de prueba unitaria del requisito 2</t>
+  </si>
+  <si>
+    <t>tests_02.py</t>
   </si>
   <si>
     <t>Codificación de requisito 3</t>
   </si>
   <si>
+    <t>Código del requisito 3</t>
+  </si>
+  <si>
     <t>Test de requisito 3</t>
   </si>
   <si>
-    <t>tests-03.py</t>
+    <t>Código de prueba unitaria del requisito 3</t>
+  </si>
+  <si>
+    <t>tests_03.py</t>
   </si>
   <si>
     <t>Elaborar Informe de Pruebas 1</t>
@@ -329,198 +344,165 @@
     <t>Ames D. (DF), Castillo C. (AJ), Cjumo J. (DF), Hinostroza G. (DB), Ipanaque J. (AS), Ramírez P. (UX), Saenz C. (DF)</t>
   </si>
   <si>
-    <t>Linea base 1</t>
-  </si>
-  <si>
     <t>Hito 1 - Fin del Iteración #1</t>
   </si>
   <si>
     <t>Verificar y actualizar la Arquitectura y Diseño del Software</t>
   </si>
   <si>
-    <t>Documento de Arquitectura del Software 2</t>
-  </si>
-  <si>
-    <t>GS-AS-02.DOCX</t>
-  </si>
-  <si>
     <t>Verificar y actualizar documento de Especificación de UI</t>
   </si>
   <si>
-    <t>Documento de Especificación de UI 2</t>
-  </si>
-  <si>
-    <t>GS-UI-02.DOCX</t>
+    <t>Verificar y actualizar la Guía de Estilos</t>
+  </si>
+  <si>
+    <t>Verificar y actualizar documento de Especificación de la Base de Datos</t>
+  </si>
+  <si>
+    <t>Verificar y actualizar Plan de Fase</t>
+  </si>
+  <si>
+    <t>Elaborar Plan de Iteración 2</t>
+  </si>
+  <si>
+    <t>Documento de Plan de Iteración 2</t>
+  </si>
+  <si>
+    <t>GS-PI-02.DOCX</t>
+  </si>
+  <si>
+    <t>Elaborar Casos de Uso 2</t>
+  </si>
+  <si>
+    <t>Documento de Casos de Uso 2</t>
+  </si>
+  <si>
+    <t>GS-CU-02.DOCX</t>
+  </si>
+  <si>
+    <t>Codificación de requisito 4</t>
+  </si>
+  <si>
+    <t>Código del requisito 4</t>
+  </si>
+  <si>
+    <t>Test de requisito 4</t>
+  </si>
+  <si>
+    <t>Código de prueba unitaria del requisito 4</t>
+  </si>
+  <si>
+    <t>tests_04.py</t>
+  </si>
+  <si>
+    <t>Codificación de requisito 5</t>
+  </si>
+  <si>
+    <t>Código del requisito 5</t>
+  </si>
+  <si>
+    <t>Ames D. (DF), Cjumo J. (DF), Hinostroza G. (DB), Saenz C. (DF)</t>
+  </si>
+  <si>
+    <t>Test de requisito 5</t>
+  </si>
+  <si>
+    <t>Código de prueba unitaria del requisito 5</t>
+  </si>
+  <si>
+    <t>tests_05.py</t>
+  </si>
+  <si>
+    <t>Elaborar Informe de Pruebas 2</t>
+  </si>
+  <si>
+    <t>Documento de Informe de Pruebas 2</t>
+  </si>
+  <si>
+    <t>GS-IP-02.DOCX</t>
+  </si>
+  <si>
+    <t>Reporte del Desarrollo del Software 2</t>
+  </si>
+  <si>
+    <t>GS-RDS-02.DOCX</t>
+  </si>
+  <si>
+    <t>Hito 2 - Fin del Iteración #2</t>
+  </si>
+  <si>
+    <t>Elaborar Plan de Iteración 3</t>
+  </si>
+  <si>
+    <t>Documento de Plan de Iteración 3</t>
+  </si>
+  <si>
+    <t>GS-PI-03.DOCX</t>
+  </si>
+  <si>
+    <t>Ames D. (DF), Castillo C. (AJ), Cjumo J. (DF), Hinostroza G. (DB), Ipanaque J. (JP), Ramírez P. (UX), Saenz C. (DF)</t>
+  </si>
+  <si>
+    <t>Elaborar Casos de Uso 3</t>
+  </si>
+  <si>
+    <t>Documento de Casos de Uso 3</t>
+  </si>
+  <si>
+    <t>GS-CU-03.DOCX</t>
+  </si>
+  <si>
+    <t>Codificación de requisito 6</t>
+  </si>
+  <si>
+    <t>Código del requisito 6</t>
+  </si>
+  <si>
+    <t>Test de requisito 6</t>
+  </si>
+  <si>
+    <t>Código de prueba unitaria del requisito 6</t>
+  </si>
+  <si>
+    <t>tests_06.py</t>
+  </si>
+  <si>
+    <t>Codificación de requisito 7</t>
+  </si>
+  <si>
+    <t>Código del requisito 7</t>
+  </si>
+  <si>
+    <t>Test de requisito 7</t>
+  </si>
+  <si>
+    <t>Código de prueba unitaria del requisito 7</t>
+  </si>
+  <si>
+    <t>tests_07.py</t>
+  </si>
+  <si>
+    <t>Elaborar Informe de Pruebas 3</t>
+  </si>
+  <si>
+    <t>Documento de Informe de Pruebas 3</t>
+  </si>
+  <si>
+    <t>GS-IP-03.DOCX</t>
+  </si>
+  <si>
+    <t>Verificar y finalizar la Arquitectura y Diseño del Software</t>
+  </si>
+  <si>
+    <t>Verificar y finalizar documento de Especificación de UI</t>
   </si>
   <si>
     <t>Verificar y finalizar la Guía de Estilos</t>
   </si>
   <si>
-    <t>Documento de Guía de Estilos 2</t>
-  </si>
-  <si>
-    <t>GS-GE-02.DOCX</t>
-  </si>
-  <si>
-    <t>Verificar y actualizar documento de Especificación de la Base de Datos</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de la BD 2</t>
-  </si>
-  <si>
-    <t>GS-DEBD-02.DOCX</t>
-  </si>
-  <si>
-    <t>Verificar y actualizar Plan de Fase</t>
-  </si>
-  <si>
-    <t>Documento de Plan de Fase 2</t>
-  </si>
-  <si>
-    <t>GS-PF-02.DOCX</t>
-  </si>
-  <si>
-    <t>Elaborar Plan de Iteración 2</t>
-  </si>
-  <si>
-    <t>Documento de Plan de Iteración 2</t>
-  </si>
-  <si>
-    <t>GS-PI-02.DOCX</t>
-  </si>
-  <si>
-    <t>Elaborar Casos de Uso 2</t>
-  </si>
-  <si>
-    <t>Documento de Casos de Uso 2</t>
-  </si>
-  <si>
-    <t>GS-CU-02.DOCX</t>
-  </si>
-  <si>
-    <t>Codificación de requisito 4</t>
-  </si>
-  <si>
-    <t>Test de requisito 4</t>
-  </si>
-  <si>
-    <t>tests-04.py</t>
-  </si>
-  <si>
-    <t>Codificación de requisito 5</t>
-  </si>
-  <si>
-    <t>Ames D. (DF), Cjumo J. (DF), Hinostroza G. (DB), Saenz C. (DF)</t>
-  </si>
-  <si>
-    <t>Test de requisito 5</t>
-  </si>
-  <si>
-    <t>tests-05.py</t>
-  </si>
-  <si>
-    <t>Elaborar Informe de Pruebas 2</t>
-  </si>
-  <si>
-    <t>Documento de Informe de Pruebas 2</t>
-  </si>
-  <si>
-    <t>GS-IP-02.DOCX</t>
-  </si>
-  <si>
-    <t>Reporte del Desarrollo del Software 2</t>
-  </si>
-  <si>
-    <t>GS-RDS-02.DOCX</t>
-  </si>
-  <si>
-    <t>Linea base 2</t>
-  </si>
-  <si>
-    <t>Hito 2 - Fin del Iteración #2</t>
-  </si>
-  <si>
-    <t>Elaborar Plan de Iteración 3</t>
-  </si>
-  <si>
-    <t>Documento de Plan de Iteración 3</t>
-  </si>
-  <si>
-    <t>GS-PI-03.DOCX</t>
-  </si>
-  <si>
-    <t>Ames D. (DF), Castillo C. (AJ), Cjumo J. (DF), Hinostroza G. (DB), Ipanaque J. (JP), Ramírez P. (UX), Saenz C. (DF)</t>
-  </si>
-  <si>
-    <t>Elaborar Casos de Uso 3</t>
-  </si>
-  <si>
-    <t>Documento de Casos de Uso 3</t>
-  </si>
-  <si>
-    <t>GS-CU-03.DOCX</t>
-  </si>
-  <si>
-    <t>Codificación de requisito 6</t>
-  </si>
-  <si>
-    <t>Test de requisito 6</t>
-  </si>
-  <si>
-    <t>tests-06.py</t>
-  </si>
-  <si>
-    <t>Codificación de requisito 7</t>
-  </si>
-  <si>
-    <t>Test de requisito 7</t>
-  </si>
-  <si>
-    <t>tests-07.py</t>
-  </si>
-  <si>
-    <t>Elaborar Informe de Pruebas 3</t>
-  </si>
-  <si>
-    <t>Documento de Informe de Pruebas 3</t>
-  </si>
-  <si>
-    <t>GS-IP-03.DOCX</t>
-  </si>
-  <si>
-    <t>Verificar y finalizar la Arquitectura y Diseño del Software</t>
-  </si>
-  <si>
-    <t>Documento de Arquitectura del Software 3</t>
-  </si>
-  <si>
-    <t>GS-AS-03.DOCX</t>
-  </si>
-  <si>
-    <t>Verificar y finalizar documento de Especificación de UI</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de UI 3</t>
-  </si>
-  <si>
-    <t>GS-UI-03.DOCX</t>
-  </si>
-  <si>
-    <t>Documento de Guía de Estilos 3</t>
-  </si>
-  <si>
-    <t>GS-GE-03.DOCX</t>
-  </si>
-  <si>
     <t>Verificar y finalizar documento de Especificación de la Base de Datos</t>
   </si>
   <si>
-    <t>Documento de Especificación de la BD 3</t>
-  </si>
-  <si>
-    <t>GS-DEBD-03.DOCX</t>
-  </si>
-  <si>
     <t>Generar documentación para el usuario</t>
   </si>
   <si>
@@ -533,12 +515,6 @@
     <t>Verificar y finalizar Plan de Fase</t>
   </si>
   <si>
-    <t>Documento de Plan de Fase 3</t>
-  </si>
-  <si>
-    <t>GS-PF-03.DOCX</t>
-  </si>
-  <si>
     <t>Reporte del Desarrollo del Software 3</t>
   </si>
   <si>
@@ -552,9 +528,6 @@
   </si>
   <si>
     <t>GS-ACP.DOCX</t>
-  </si>
-  <si>
-    <t>Linea base 3</t>
   </si>
   <si>
     <t>Hito 3 - Fin del Iteración #3</t>
@@ -713,12 +686,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <i/>
       <color theme="1"/>
-      <name val="&quot;Helvetica Neue&quot;"/>
-    </font>
-    <font>
-      <i/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
@@ -744,6 +712,9 @@
     </font>
     <font>
       <color rgb="FFFFFFFF"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
@@ -874,7 +845,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -961,7 +932,7 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="7" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="7" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -984,52 +955,58 @@
     <xf borderId="5" fillId="8" fontId="11" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="4" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="4" fillId="7" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="7" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="3" fillId="5" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="5" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="20" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="5" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="3" fillId="6" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="7" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="6" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="7" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="7" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="7" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="4" fillId="5" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="4" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="24" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="5" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="7" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="7" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1279,7 +1256,7 @@
     <col customWidth="1" min="1" max="1" width="12.0"/>
     <col customWidth="1" min="2" max="2" width="70.25"/>
     <col customWidth="1" min="3" max="3" width="76.13"/>
-    <col customWidth="1" min="4" max="4" width="15.63"/>
+    <col customWidth="1" min="4" max="4" width="18.0"/>
     <col customWidth="1" min="5" max="5" width="97.25"/>
     <col customWidth="1" min="6" max="6" width="22.13"/>
     <col customWidth="1" min="7" max="7" width="21.63"/>
@@ -1843,14 +1820,14 @@
       <c r="B28" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="17" t="s">
+      <c r="C28" s="24" t="s">
         <v>80</v>
       </c>
+      <c r="D28" s="37" t="s">
+        <v>81</v>
+      </c>
       <c r="E28" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F28" s="20">
         <v>45036.0</v>
@@ -1865,16 +1842,16 @@
     <row r="29">
       <c r="A29" s="5"/>
       <c r="B29" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="37" t="s">
         <v>83</v>
       </c>
+      <c r="C29" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>85</v>
+      </c>
       <c r="E29" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F29" s="20">
         <v>45044.0</v>
@@ -1889,16 +1866,16 @@
     <row r="30">
       <c r="A30" s="5"/>
       <c r="B30" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>81</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F30" s="20">
         <v>45036.0</v>
@@ -1913,16 +1890,16 @@
     <row r="31">
       <c r="A31" s="5"/>
       <c r="B31" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="37" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>91</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F31" s="20">
         <v>45044.0</v>
@@ -1937,16 +1914,16 @@
     <row r="32">
       <c r="A32" s="5"/>
       <c r="B32" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>86</v>
+        <v>92</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>81</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F32" s="20">
         <v>45036.0</v>
@@ -1961,16 +1938,16 @@
     <row r="33">
       <c r="A33" s="5"/>
       <c r="B33" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="38" t="s">
-        <v>91</v>
+        <v>94</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>96</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F33" s="20">
         <v>45044.0</v>
@@ -1985,16 +1962,16 @@
     <row r="34">
       <c r="A34" s="5"/>
       <c r="B34" s="16" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F34" s="20">
         <v>45046.0</v>
@@ -2009,16 +1986,16 @@
     <row r="35">
       <c r="A35" s="5"/>
       <c r="B35" s="16" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F35" s="20">
         <v>45046.0</v>
@@ -2031,31 +2008,29 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="40"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="43">
+      <c r="A36" s="26"/>
+      <c r="B36" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="41"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="44">
         <v>45046.0</v>
       </c>
-      <c r="H36" s="42"/>
+      <c r="H36" s="43"/>
     </row>
     <row r="37">
       <c r="A37" s="5"/>
       <c r="B37" s="16" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>37</v>
@@ -2066,20 +2041,20 @@
       <c r="G37" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H37" s="21">
-        <v>0.0</v>
+      <c r="H37" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="5"/>
-      <c r="B38" s="44" t="s">
-        <v>104</v>
+      <c r="B38" s="46" t="s">
+        <v>106</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>41</v>
@@ -2090,8 +2065,8 @@
       <c r="G38" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H38" s="21">
-        <v>0.0</v>
+      <c r="H38" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="39">
@@ -2100,10 +2075,10 @@
         <v>107</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>41</v>
@@ -2114,20 +2089,20 @@
       <c r="G39" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H39" s="21">
-        <v>0.0</v>
+      <c r="H39" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="5"/>
-      <c r="B40" s="44" t="s">
-        <v>110</v>
+      <c r="B40" s="46" t="s">
+        <v>108</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>112</v>
+        <v>47</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>48</v>
@@ -2138,20 +2113,20 @@
       <c r="G40" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H40" s="21">
-        <v>0.0</v>
+      <c r="H40" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="5"/>
       <c r="B41" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>114</v>
+        <v>26</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>18</v>
@@ -2162,20 +2137,20 @@
       <c r="G41" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H41" s="21">
-        <v>0.0</v>
+      <c r="H41" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="5"/>
       <c r="B42" s="16" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>18</v>
@@ -2186,20 +2161,20 @@
       <c r="G42" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H42" s="21">
-        <v>0.0</v>
+      <c r="H42" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="5"/>
       <c r="B43" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="C43" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>121</v>
+        <v>113</v>
+      </c>
+      <c r="C43" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="48" t="s">
+        <v>115</v>
       </c>
       <c r="E43" s="30" t="s">
         <v>78</v>
@@ -2210,23 +2185,23 @@
       <c r="G43" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H43" s="46">
-        <v>0.0</v>
+      <c r="H43" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="5"/>
       <c r="B44" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>86</v>
+        <v>116</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>81</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F44" s="20">
         <v>45056.0</v>
@@ -2234,23 +2209,23 @@
       <c r="G44" s="20">
         <v>45065.0</v>
       </c>
-      <c r="H44" s="21">
-        <v>0.0</v>
+      <c r="H44" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="5"/>
       <c r="B45" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" s="37" t="s">
-        <v>124</v>
+        <v>118</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="38" t="s">
+        <v>120</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F45" s="20">
         <v>45066.0</v>
@@ -2258,23 +2233,23 @@
       <c r="G45" s="20">
         <v>45067.0</v>
       </c>
-      <c r="H45" s="21">
-        <v>0.0</v>
+      <c r="H45" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="5"/>
       <c r="B46" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>80</v>
+        <v>121</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" s="37" t="s">
+        <v>81</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F46" s="20">
         <v>45056.0</v>
@@ -2282,23 +2257,23 @@
       <c r="G46" s="20">
         <v>45065.0</v>
       </c>
-      <c r="H46" s="21">
-        <v>0.0</v>
+      <c r="H46" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="5"/>
       <c r="B47" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" s="37" t="s">
-        <v>128</v>
+        <v>124</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D47" s="38" t="s">
+        <v>126</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F47" s="20">
         <v>45066.0</v>
@@ -2306,23 +2281,23 @@
       <c r="G47" s="20">
         <v>45067.0</v>
       </c>
-      <c r="H47" s="21">
-        <v>0.0</v>
+      <c r="H47" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="5"/>
       <c r="B48" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C48" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>131</v>
-      </c>
       <c r="E48" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F48" s="20">
         <v>45068.0</v>
@@ -2331,22 +2306,22 @@
         <v>45069.0</v>
       </c>
       <c r="H48" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="5"/>
       <c r="B49" s="16" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F49" s="20">
         <v>45069.0</v>
@@ -2355,38 +2330,36 @@
         <v>45070.0</v>
       </c>
       <c r="H49" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="B50" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="C50" s="47"/>
-      <c r="D50" s="48"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="43">
+      <c r="A50" s="26"/>
+      <c r="B50" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="49"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="44">
         <v>45070.0</v>
       </c>
-      <c r="H50" s="50"/>
+      <c r="H50" s="52"/>
     </row>
     <row r="51">
       <c r="A51" s="5"/>
       <c r="B51" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" s="19" t="s">
         <v>136</v>
-      </c>
-      <c r="C51" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D51" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>139</v>
       </c>
       <c r="F51" s="20">
         <v>45070.0</v>
@@ -2401,13 +2374,13 @@
     <row r="52">
       <c r="A52" s="5"/>
       <c r="B52" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="D52" s="51" t="s">
-        <v>142</v>
+        <v>138</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>139</v>
       </c>
       <c r="E52" s="19" t="s">
         <v>78</v>
@@ -2425,16 +2398,16 @@
     <row r="53">
       <c r="A53" s="5"/>
       <c r="B53" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>80</v>
+        <v>140</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" s="37" t="s">
+        <v>81</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F53" s="20">
         <v>45076.0</v>
@@ -2449,16 +2422,16 @@
     <row r="54">
       <c r="A54" s="5"/>
       <c r="B54" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="D54" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="C54" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" s="37" t="s">
-        <v>145</v>
-      </c>
       <c r="E54" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F54" s="20">
         <v>45089.0</v>
@@ -2473,16 +2446,16 @@
     <row r="55">
       <c r="A55" s="5"/>
       <c r="B55" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="C55" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>80</v>
+      <c r="D55" s="37" t="s">
+        <v>81</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F55" s="20">
         <v>45076.0</v>
@@ -2499,14 +2472,14 @@
       <c r="B56" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C56" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="37" t="s">
+      <c r="C56" s="24" t="s">
         <v>148</v>
       </c>
+      <c r="D56" s="53" t="s">
+        <v>149</v>
+      </c>
       <c r="E56" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F56" s="20">
         <v>45089.0</v>
@@ -2521,16 +2494,16 @@
     <row r="57">
       <c r="A57" s="5"/>
       <c r="B57" s="16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F57" s="20">
         <v>45092.0</v>
@@ -2545,13 +2518,13 @@
     <row r="58">
       <c r="A58" s="5"/>
       <c r="B58" s="16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>153</v>
+        <v>35</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>154</v>
+        <v>36</v>
       </c>
       <c r="E58" s="19" t="s">
         <v>37</v>
@@ -2568,14 +2541,14 @@
     </row>
     <row r="59">
       <c r="A59" s="5"/>
-      <c r="B59" s="44" t="s">
-        <v>155</v>
+      <c r="B59" s="46" t="s">
+        <v>154</v>
       </c>
       <c r="C59" s="32" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>157</v>
+        <v>40</v>
       </c>
       <c r="E59" s="19" t="s">
         <v>41</v>
@@ -2593,13 +2566,13 @@
     <row r="60">
       <c r="A60" s="5"/>
       <c r="B60" s="16" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="C60" s="25" t="s">
-        <v>158</v>
+        <v>43</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>159</v>
+        <v>44</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>41</v>
@@ -2616,14 +2589,14 @@
     </row>
     <row r="61">
       <c r="A61" s="5"/>
-      <c r="B61" s="44" t="s">
-        <v>160</v>
+      <c r="B61" s="46" t="s">
+        <v>156</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>161</v>
+        <v>46</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>162</v>
+        <v>47</v>
       </c>
       <c r="E61" s="19" t="s">
         <v>48</v>
@@ -2641,13 +2614,13 @@
     <row r="62">
       <c r="A62" s="5"/>
       <c r="B62" s="16" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C62" s="25" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E62" s="19" t="s">
         <v>41</v>
@@ -2665,16 +2638,16 @@
     <row r="63">
       <c r="A63" s="5"/>
       <c r="B63" s="16" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>167</v>
+        <v>26</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>168</v>
+        <v>27</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F63" s="20">
         <v>45094.0</v>
@@ -2689,16 +2662,16 @@
     <row r="64">
       <c r="A64" s="5"/>
       <c r="B64" s="16" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F64" s="20">
         <v>45094.0</v>
@@ -2713,16 +2686,16 @@
     <row r="65">
       <c r="A65" s="5"/>
       <c r="B65" s="16" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C65" s="25" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F65" s="20">
         <v>45096.0</v>
@@ -2735,20 +2708,18 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="B66" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="C66" s="52"/>
-      <c r="D66" s="42"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43">
+      <c r="A66" s="26"/>
+      <c r="B66" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="C66" s="54"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="44">
         <v>45098.0</v>
       </c>
-      <c r="H66" s="50"/>
+      <c r="H66" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2757,7 +2728,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="D33"/>
+    <hyperlink r:id="rId2" ref="D56"/>
   </hyperlinks>
   <drawing r:id="rId3"/>
 </worksheet>
@@ -2778,79 +2749,79 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3">
+      <c r="B3" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="B4" s="57" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="60" t="s">
         <v>176</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3">
-      <c r="B3" s="54" t="s">
+    </row>
+    <row r="8">
+      <c r="B8" s="61" t="s">
         <v>177</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4">
-      <c r="B4" s="55" t="s">
+      <c r="C8" s="60" t="s">
         <v>178</v>
       </c>
-      <c r="C4" s="56" t="s">
+    </row>
+    <row r="9">
+      <c r="B9" s="59" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="57" t="s">
+      <c r="C9" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="C5" s="58" t="s">
+    </row>
+    <row r="10">
+      <c r="B10" s="59" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="57" t="s">
+      <c r="C10" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="58" t="s">
+    </row>
+    <row r="11">
+      <c r="B11" s="59" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="57" t="s">
+      <c r="C11" s="60" t="s">
         <v>184</v>
-      </c>
-      <c r="C7" s="58" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="59" t="s">
-        <v>186</v>
-      </c>
-      <c r="C8" s="58" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="57" t="s">
-        <v>188</v>
-      </c>
-      <c r="C9" s="60" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="57" t="s">
-        <v>190</v>
-      </c>
-      <c r="C10" s="58" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="57" t="s">
-        <v>192</v>
-      </c>
-      <c r="C11" s="58" t="s">
-        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se finaliza el cronograma de proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/GoShop/Documentos/GS-CP.xlsx
+++ b/Desarrollo/GoShop/Documentos/GS-CP.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="199">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -92,7 +92,7 @@
     <t>Desarrollar del Plan de Proyecto</t>
   </si>
   <si>
-    <t>Plan de Proyecto (PROJECT CHARTER)</t>
+    <t>Plan de Proyecto</t>
   </si>
   <si>
     <t>GS-PP.DOCX</t>
@@ -452,6 +452,24 @@
     <t>GS-CU-03.DOCX</t>
   </si>
   <si>
+    <t>Actualización de Casos de Uso 2</t>
+  </si>
+  <si>
+    <t>Actualización de Plan de Proyecto</t>
+  </si>
+  <si>
+    <t>Actualización de especificación de requisitos 1</t>
+  </si>
+  <si>
+    <t>Actualización de especificación de requisitos 5</t>
+  </si>
+  <si>
+    <t>Actualización de especificación de requisitos 6</t>
+  </si>
+  <si>
+    <t>Actualización de especificación de requisitos 7</t>
+  </si>
+  <si>
     <t>Codificación de requisito 6</t>
   </si>
   <si>
@@ -482,6 +500,21 @@
     <t>tests_07.py</t>
   </si>
   <si>
+    <t>Actualización de test de requisito 1</t>
+  </si>
+  <si>
+    <t>Actualización de test de requisito 2</t>
+  </si>
+  <si>
+    <t>Actualización de test de requisito 3</t>
+  </si>
+  <si>
+    <t>Actualización de test de requisito 4</t>
+  </si>
+  <si>
+    <t>Actualización de test de requisito 5</t>
+  </si>
+  <si>
     <t>Elaborar Informe de Pruebas 3</t>
   </si>
   <si>
@@ -512,6 +545,9 @@
     <t>GS-MU.DOCX</t>
   </si>
   <si>
+    <t>Ames D. (DF), Castillo C. (T),Hinostroza G. (DB), Ramírez P. (UX), Saenz C. (DF)</t>
+  </si>
+  <si>
     <t>Verificar y finalizar Plan de Fase</t>
   </si>
   <si>
@@ -528,6 +564,12 @@
   </si>
   <si>
     <t>GS-ACP.DOCX</t>
+  </si>
+  <si>
+    <t>Finalización de cronograma de proyecto</t>
+  </si>
+  <si>
+    <t>Cronograma del proyecto</t>
   </si>
   <si>
     <t>Hito 3 - Fin del Iteración #3</t>
@@ -910,7 +952,7 @@
     <xf borderId="4" fillId="7" fontId="11" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="7" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -919,9 +961,6 @@
     <xf borderId="4" fillId="7" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="7" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1004,6 +1043,9 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="7" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="5" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1253,7 +1295,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.0"/>
+    <col customWidth="1" min="1" max="1" width="3.38"/>
     <col customWidth="1" min="2" max="2" width="70.25"/>
     <col customWidth="1" min="3" max="3" width="76.13"/>
     <col customWidth="1" min="4" max="4" width="18.0"/>
@@ -1460,7 +1502,7 @@
       <c r="B13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="18" t="s">
@@ -1484,7 +1526,7 @@
       <c r="B14" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="22" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="18" t="s">
@@ -1508,7 +1550,7 @@
       <c r="B15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="22" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="18" t="s">
@@ -1528,23 +1570,23 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="30">
         <v>45026.0</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="30">
         <v>45046.0</v>
       </c>
       <c r="H16" s="21">
@@ -1552,11 +1594,11 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="22" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -1576,11 +1618,11 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="22" t="s">
         <v>43</v>
       </c>
       <c r="D18" s="18" t="s">
@@ -1600,11 +1642,11 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="26"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="31" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="18" t="s">
@@ -1624,11 +1666,11 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="22" t="s">
         <v>50</v>
       </c>
       <c r="D20" s="18" t="s">
@@ -1649,10 +1691,10 @@
     </row>
     <row r="21">
       <c r="A21" s="5"/>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="33" t="s">
         <v>54</v>
       </c>
       <c r="D21" s="18" t="s">
@@ -1673,10 +1715,10 @@
     </row>
     <row r="22">
       <c r="A22" s="5"/>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="33" t="s">
         <v>58</v>
       </c>
       <c r="D22" s="18" t="s">
@@ -1697,10 +1739,10 @@
     </row>
     <row r="23">
       <c r="A23" s="5"/>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="33" t="s">
         <v>62</v>
       </c>
       <c r="D23" s="18" t="s">
@@ -1721,10 +1763,10 @@
     </row>
     <row r="24">
       <c r="A24" s="5"/>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="33" t="s">
         <v>66</v>
       </c>
       <c r="D24" s="18" t="s">
@@ -1745,19 +1787,19 @@
     </row>
     <row r="25">
       <c r="A25" s="5"/>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="33" t="s">
         <v>69</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="35" t="s">
+      <c r="E25" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="F25" s="36">
+      <c r="F25" s="35">
         <v>45033.0</v>
       </c>
       <c r="G25" s="20">
@@ -1769,10 +1811,10 @@
     </row>
     <row r="26">
       <c r="A26" s="5"/>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="33" t="s">
         <v>73</v>
       </c>
       <c r="D26" s="18" t="s">
@@ -1781,7 +1823,7 @@
       <c r="E26" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="36">
+      <c r="F26" s="35">
         <v>45033.0</v>
       </c>
       <c r="G26" s="20">
@@ -1796,7 +1838,7 @@
       <c r="B27" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="22" t="s">
         <v>76</v>
       </c>
       <c r="D27" s="18" t="s">
@@ -1823,7 +1865,7 @@
       <c r="C28" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="36" t="s">
         <v>81</v>
       </c>
       <c r="E28" s="19" t="s">
@@ -1847,7 +1889,7 @@
       <c r="C29" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="37" t="s">
         <v>85</v>
       </c>
       <c r="E29" s="19" t="s">
@@ -1871,7 +1913,7 @@
       <c r="C30" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="36" t="s">
         <v>81</v>
       </c>
       <c r="E30" s="19" t="s">
@@ -1895,7 +1937,7 @@
       <c r="C31" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="37" t="s">
         <v>91</v>
       </c>
       <c r="E31" s="19" t="s">
@@ -1919,7 +1961,7 @@
       <c r="C32" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="36" t="s">
         <v>81</v>
       </c>
       <c r="E32" s="19" t="s">
@@ -1943,7 +1985,7 @@
       <c r="C33" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="39" t="s">
+      <c r="D33" s="38" t="s">
         <v>96</v>
       </c>
       <c r="E33" s="19" t="s">
@@ -1964,7 +2006,7 @@
       <c r="B34" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="22" t="s">
         <v>98</v>
       </c>
       <c r="D34" s="18" t="s">
@@ -1988,7 +2030,7 @@
       <c r="B35" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="22" t="s">
         <v>101</v>
       </c>
       <c r="D35" s="18" t="s">
@@ -2008,25 +2050,25 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="26"/>
-      <c r="B36" s="40" t="s">
+      <c r="A36" s="25"/>
+      <c r="B36" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44">
+      <c r="C36" s="40"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="43">
         <v>45046.0</v>
       </c>
-      <c r="H36" s="43"/>
+      <c r="H36" s="42"/>
     </row>
     <row r="37">
       <c r="A37" s="5"/>
       <c r="B37" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="22" t="s">
         <v>35</v>
       </c>
       <c r="D37" s="18" t="s">
@@ -2041,16 +2083,16 @@
       <c r="G37" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H37" s="45">
+      <c r="H37" s="44">
         <v>1.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="5"/>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="22" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="18" t="s">
@@ -2065,7 +2107,7 @@
       <c r="G38" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H38" s="45">
+      <c r="H38" s="44">
         <v>1.0</v>
       </c>
     </row>
@@ -2074,7 +2116,7 @@
       <c r="B39" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="22" t="s">
         <v>43</v>
       </c>
       <c r="D39" s="18" t="s">
@@ -2089,16 +2131,16 @@
       <c r="G39" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H39" s="45">
+      <c r="H39" s="44">
         <v>1.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="5"/>
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="31" t="s">
         <v>46</v>
       </c>
       <c r="D40" s="18" t="s">
@@ -2113,7 +2155,7 @@
       <c r="G40" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H40" s="45">
+      <c r="H40" s="44">
         <v>1.0</v>
       </c>
     </row>
@@ -2122,7 +2164,7 @@
       <c r="B41" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="18" t="s">
@@ -2137,7 +2179,7 @@
       <c r="G41" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H41" s="45">
+      <c r="H41" s="44">
         <v>1.0</v>
       </c>
     </row>
@@ -2146,7 +2188,7 @@
       <c r="B42" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="22" t="s">
         <v>111</v>
       </c>
       <c r="D42" s="18" t="s">
@@ -2161,22 +2203,22 @@
       <c r="G42" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H42" s="45">
+      <c r="H42" s="44">
         <v>1.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="5"/>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="47" t="s">
+      <c r="C43" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="D43" s="48" t="s">
+      <c r="D43" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="E43" s="30" t="s">
+      <c r="E43" s="29" t="s">
         <v>78</v>
       </c>
       <c r="F43" s="20">
@@ -2185,7 +2227,7 @@
       <c r="G43" s="20">
         <v>45056.0</v>
       </c>
-      <c r="H43" s="45">
+      <c r="H43" s="44">
         <v>1.0</v>
       </c>
     </row>
@@ -2197,7 +2239,7 @@
       <c r="C44" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="D44" s="37" t="s">
+      <c r="D44" s="36" t="s">
         <v>81</v>
       </c>
       <c r="E44" s="19" t="s">
@@ -2209,7 +2251,7 @@
       <c r="G44" s="20">
         <v>45065.0</v>
       </c>
-      <c r="H44" s="45">
+      <c r="H44" s="44">
         <v>1.0</v>
       </c>
     </row>
@@ -2221,7 +2263,7 @@
       <c r="C45" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="D45" s="38" t="s">
+      <c r="D45" s="37" t="s">
         <v>120</v>
       </c>
       <c r="E45" s="19" t="s">
@@ -2233,7 +2275,7 @@
       <c r="G45" s="20">
         <v>45067.0</v>
       </c>
-      <c r="H45" s="45">
+      <c r="H45" s="44">
         <v>1.0</v>
       </c>
     </row>
@@ -2245,7 +2287,7 @@
       <c r="C46" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="D46" s="37" t="s">
+      <c r="D46" s="36" t="s">
         <v>81</v>
       </c>
       <c r="E46" s="19" t="s">
@@ -2257,7 +2299,7 @@
       <c r="G46" s="20">
         <v>45065.0</v>
       </c>
-      <c r="H46" s="45">
+      <c r="H46" s="44">
         <v>1.0</v>
       </c>
     </row>
@@ -2269,7 +2311,7 @@
       <c r="C47" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="D47" s="38" t="s">
+      <c r="D47" s="37" t="s">
         <v>126</v>
       </c>
       <c r="E47" s="19" t="s">
@@ -2281,7 +2323,7 @@
       <c r="G47" s="20">
         <v>45067.0</v>
       </c>
-      <c r="H47" s="45">
+      <c r="H47" s="44">
         <v>1.0</v>
       </c>
     </row>
@@ -2290,7 +2332,7 @@
       <c r="B48" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="22" t="s">
         <v>128</v>
       </c>
       <c r="D48" s="18" t="s">
@@ -2314,7 +2356,7 @@
       <c r="B49" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="22" t="s">
         <v>130</v>
       </c>
       <c r="D49" s="18" t="s">
@@ -2334,25 +2376,25 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="26"/>
-      <c r="B50" s="40" t="s">
+      <c r="A50" s="25"/>
+      <c r="B50" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="C50" s="49"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="44">
+      <c r="C50" s="48"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="43">
         <v>45070.0</v>
       </c>
-      <c r="H50" s="52"/>
+      <c r="H50" s="51"/>
     </row>
     <row r="51">
       <c r="A51" s="5"/>
       <c r="B51" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="22" t="s">
         <v>134</v>
       </c>
       <c r="D51" s="18" t="s">
@@ -2365,10 +2407,10 @@
         <v>45070.0</v>
       </c>
       <c r="G51" s="20">
-        <v>45076.0</v>
+        <v>45077.0</v>
       </c>
       <c r="H51" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="52">
@@ -2376,23 +2418,23 @@
       <c r="B52" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C52" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D52" s="29" t="s">
+      <c r="D52" s="28" t="s">
         <v>139</v>
       </c>
       <c r="E52" s="19" t="s">
         <v>78</v>
       </c>
       <c r="F52" s="20">
-        <v>45101.0</v>
+        <v>45077.0</v>
       </c>
       <c r="G52" s="20">
-        <v>45076.0</v>
+        <v>45085.0</v>
       </c>
       <c r="H52" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="53">
@@ -2400,326 +2442,614 @@
       <c r="B53" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="C53" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="D53" s="37" t="s">
-        <v>81</v>
+      <c r="C53" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>115</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>123</v>
+        <v>78</v>
       </c>
       <c r="F53" s="20">
-        <v>45076.0</v>
+        <v>45077.0</v>
       </c>
       <c r="G53" s="20">
-        <v>45088.0</v>
+        <v>45085.0</v>
       </c>
       <c r="H53" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="5"/>
       <c r="B54" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="D54" s="38" t="s">
-        <v>144</v>
+        <v>141</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="F54" s="20">
-        <v>45089.0</v>
+        <v>45077.0</v>
       </c>
       <c r="G54" s="20">
-        <v>45091.0</v>
+        <v>45085.0</v>
       </c>
       <c r="H54" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="5"/>
       <c r="B55" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="D55" s="37" t="s">
-        <v>81</v>
+        <v>142</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
       <c r="F55" s="20">
-        <v>45076.0</v>
+        <v>45077.0</v>
       </c>
       <c r="G55" s="20">
-        <v>45088.0</v>
+        <v>45085.0</v>
       </c>
       <c r="H55" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="5"/>
       <c r="B56" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D56" s="53" t="s">
-        <v>149</v>
+        <v>143</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="F56" s="20">
-        <v>45089.0</v>
+        <v>45077.0</v>
       </c>
       <c r="G56" s="20">
-        <v>45091.0</v>
+        <v>45085.0</v>
       </c>
       <c r="H56" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="5"/>
       <c r="B57" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="C57" s="25" t="s">
-        <v>151</v>
+        <v>144</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>69</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>86</v>
+        <v>70</v>
+      </c>
+      <c r="E57" s="34" t="s">
+        <v>71</v>
       </c>
       <c r="F57" s="20">
-        <v>45092.0</v>
+        <v>45077.0</v>
       </c>
       <c r="G57" s="20">
-        <v>45093.0</v>
+        <v>45085.0</v>
       </c>
       <c r="H57" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="5"/>
       <c r="B58" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C58" s="25" t="s">
-        <v>35</v>
+        <v>145</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>73</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F58" s="20">
-        <v>45094.0</v>
+        <v>45077.0</v>
       </c>
       <c r="G58" s="20">
-        <v>45096.0</v>
+        <v>45085.0</v>
       </c>
       <c r="H58" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="5"/>
-      <c r="B59" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="C59" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>40</v>
+      <c r="B59" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D59" s="36" t="s">
+        <v>81</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="F59" s="20">
-        <v>45094.0</v>
+        <v>45085.0</v>
       </c>
       <c r="G59" s="20">
-        <v>45096.0</v>
+        <v>45088.0</v>
       </c>
       <c r="H59" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="5"/>
       <c r="B60" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C60" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>44</v>
+        <v>148</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D60" s="37" t="s">
+        <v>150</v>
       </c>
       <c r="E60" s="19" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="F60" s="20">
-        <v>45094.0</v>
+        <v>45089.0</v>
       </c>
       <c r="G60" s="20">
-        <v>45096.0</v>
+        <v>45091.0</v>
       </c>
       <c r="H60" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="5"/>
-      <c r="B61" s="46" t="s">
-        <v>156</v>
-      </c>
-      <c r="C61" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="D61" s="18" t="s">
-        <v>47</v>
+      <c r="B61" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D61" s="36" t="s">
+        <v>81</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>48</v>
+        <v>123</v>
       </c>
       <c r="F61" s="20">
-        <v>45094.0</v>
+        <v>45085.0</v>
       </c>
       <c r="G61" s="20">
-        <v>45096.0</v>
+        <v>45088.0</v>
       </c>
       <c r="H61" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="5"/>
       <c r="B62" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C62" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>159</v>
+        <v>153</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D62" s="52" t="s">
+        <v>155</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="F62" s="20">
-        <v>45094.0</v>
+        <v>45089.0</v>
       </c>
       <c r="G62" s="20">
-        <v>45096.0</v>
+        <v>45091.0</v>
       </c>
       <c r="H62" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="5"/>
       <c r="B63" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C63" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D63" s="18" t="s">
-        <v>27</v>
+        <v>156</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D63" s="53" t="s">
+        <v>85</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="F63" s="20">
-        <v>45094.0</v>
+        <v>45089.0</v>
       </c>
       <c r="G63" s="20">
-        <v>45096.0</v>
+        <v>45091.0</v>
       </c>
       <c r="H63" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="5"/>
       <c r="B64" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C64" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>162</v>
+        <v>157</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" s="53" t="s">
+        <v>91</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="F64" s="20">
-        <v>45094.0</v>
+        <v>45089.0</v>
       </c>
       <c r="G64" s="20">
-        <v>45096.0</v>
+        <v>45091.0</v>
       </c>
       <c r="H64" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="5"/>
       <c r="B65" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C65" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D65" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F65" s="20">
+        <v>45089.0</v>
+      </c>
+      <c r="G65" s="20">
+        <v>45091.0</v>
+      </c>
+      <c r="H65" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="5"/>
+      <c r="B66" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C66" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D66" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F66" s="20">
+        <v>45089.0</v>
+      </c>
+      <c r="G66" s="20">
+        <v>45091.0</v>
+      </c>
+      <c r="H66" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="5"/>
+      <c r="B67" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D67" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F67" s="20">
+        <v>45089.0</v>
+      </c>
+      <c r="G67" s="20">
+        <v>45091.0</v>
+      </c>
+      <c r="H67" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="5"/>
+      <c r="B68" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="D68" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="C65" s="25" t="s">
+      <c r="E68" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F68" s="20">
+        <v>45092.0</v>
+      </c>
+      <c r="G68" s="20">
+        <v>45093.0</v>
+      </c>
+      <c r="H68" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="5"/>
+      <c r="B69" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="D65" s="18" t="s">
+      <c r="C69" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F69" s="20">
+        <v>45094.0</v>
+      </c>
+      <c r="G69" s="20">
+        <v>45098.0</v>
+      </c>
+      <c r="H69" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="5"/>
+      <c r="B70" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="E65" s="19" t="s">
+      <c r="C70" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F70" s="20">
+        <v>45094.0</v>
+      </c>
+      <c r="G70" s="20">
+        <v>45098.0</v>
+      </c>
+      <c r="H70" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="5"/>
+      <c r="B71" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F71" s="20">
+        <v>45094.0</v>
+      </c>
+      <c r="G71" s="20">
+        <v>45098.0</v>
+      </c>
+      <c r="H71" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="5"/>
+      <c r="B72" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="C72" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F72" s="20">
+        <v>45094.0</v>
+      </c>
+      <c r="G72" s="20">
+        <v>45098.0</v>
+      </c>
+      <c r="H72" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="5"/>
+      <c r="B73" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="F73" s="20">
+        <v>45094.0</v>
+      </c>
+      <c r="G73" s="20">
+        <v>45098.0</v>
+      </c>
+      <c r="H73" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="5"/>
+      <c r="B74" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F74" s="20">
+        <v>45094.0</v>
+      </c>
+      <c r="G74" s="20">
+        <v>45098.0</v>
+      </c>
+      <c r="H74" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="5"/>
+      <c r="B75" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E75" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="F65" s="20">
-        <v>45096.0</v>
-      </c>
-      <c r="G65" s="20">
+      <c r="F75" s="20">
+        <v>45094.0</v>
+      </c>
+      <c r="G75" s="20">
         <v>45098.0</v>
       </c>
-      <c r="H65" s="21">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="26"/>
-      <c r="B66" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="C66" s="54"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="42"/>
-      <c r="F66" s="44"/>
-      <c r="G66" s="44">
+      <c r="H75" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="5"/>
+      <c r="B76" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F76" s="20">
+        <v>45097.0</v>
+      </c>
+      <c r="G76" s="20">
         <v>45098.0</v>
       </c>
-      <c r="H66" s="52"/>
+      <c r="H76" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="25"/>
+      <c r="B77" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F77" s="20">
+        <v>45097.0</v>
+      </c>
+      <c r="G77" s="20">
+        <v>45098.0</v>
+      </c>
+      <c r="H77" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="25"/>
+      <c r="B78" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="C78" s="54"/>
+      <c r="D78" s="42"/>
+      <c r="E78" s="41"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="43">
+        <v>45098.0</v>
+      </c>
+      <c r="H78" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2728,9 +3058,14 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="D56"/>
+    <hyperlink r:id="rId2" ref="D62"/>
+    <hyperlink r:id="rId3" ref="D63"/>
+    <hyperlink r:id="rId4" ref="D64"/>
+    <hyperlink r:id="rId5" ref="D65"/>
+    <hyperlink r:id="rId6" ref="D66"/>
+    <hyperlink r:id="rId7" ref="D67"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2750,78 +3085,78 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="55" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3">
       <c r="B3" s="56" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4">
       <c r="B4" s="57" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="59" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="C5" s="60" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="59" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="C6" s="60" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="59" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="C7" s="60" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="61" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="C8" s="60" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="59" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="C9" s="62" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="59" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="59" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="C11" s="60" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>